<commit_message>
Update Final Result - Exp1
</commit_message>
<xml_diff>
--- a/experiment1_analysis/Event_Experiment1.xlsx
+++ b/experiment1_analysis/Event_Experiment1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Eye_Tracking_Education_Video\experiment1_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5310825-A1B9-4579-BE89-522D67AF474E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27DB78F5-52DA-4D8D-B5CE-A26640776816}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{AD5F7C67-FBCE-401D-ACFA-D2AAF9955749}"/>
+    <workbookView xWindow="3432" yWindow="2412" windowWidth="17280" windowHeight="8880" xr2:uid="{AD5F7C67-FBCE-401D-ACFA-D2AAF9955749}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -422,8 +422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21ABEB11-2D2B-4FE5-9870-ED730AFF1E1D}">
   <dimension ref="A1:D141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>

</xml_diff>